<commit_message>
added total votes for pair
</commit_message>
<xml_diff>
--- a/qNa.xlsx
+++ b/qNa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\nodeJS Projects\question-game-mongo\question-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8E7190-75D3-4249-89FB-7028AE1E049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452E3474-7C1E-4946-BFBF-3850DCEEAF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B5493750-8CEC-4764-89FF-16A24E89CE02}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
   <si>
     <t>you could go to dinner with one of them</t>
   </si>
@@ -105,9 +105,6 @@
     <t>questionID</t>
   </si>
   <si>
-    <t>you could have a superpower</t>
-  </si>
-  <si>
     <t>Kamala Harris</t>
   </si>
   <si>
@@ -198,24 +195,6 @@
     <t>solstice</t>
   </si>
   <si>
-    <t>Invisibility</t>
-  </si>
-  <si>
-    <t>invisible</t>
-  </si>
-  <si>
-    <t>Flying</t>
-  </si>
-  <si>
-    <t>flying</t>
-  </si>
-  <si>
-    <t>Time Travel</t>
-  </si>
-  <si>
-    <t>timetravel</t>
-  </si>
-  <si>
     <t>you could buy one car with memecoin profits</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>mev</t>
   </si>
   <si>
-    <t>you could choose the next Binance listing?</t>
-  </si>
-  <si>
     <t>Griffain</t>
   </si>
   <si>
@@ -343,6 +319,42 @@
   </si>
   <si>
     <t>mrpunk</t>
+  </si>
+  <si>
+    <t>you could choose the next Binance listing</t>
+  </si>
+  <si>
+    <t>one of them was more likely to launch a rug</t>
+  </si>
+  <si>
+    <t>Ronaldo</t>
+  </si>
+  <si>
+    <t>cristiano</t>
+  </si>
+  <si>
+    <t>Sophie Rain</t>
+  </si>
+  <si>
+    <t>sophie</t>
+  </si>
+  <si>
+    <t>Livvy Dune</t>
+  </si>
+  <si>
+    <t>livvy</t>
+  </si>
+  <si>
+    <t>Mr. Beast</t>
+  </si>
+  <si>
+    <t>mrBeast</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>Ishowspeed</t>
   </si>
 </sst>
 </file>
@@ -723,7 +735,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +781,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C8" si="0">_xlfn.CONCAT("Q",A3)</f>
@@ -786,7 +798,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>95</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -794,7 +806,7 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v>wat &lt;span class='ifOrangeColor'&gt;$if&lt;/span&gt; you could have a superpower?</v>
+        <v>wat &lt;span class='ifOrangeColor'&gt;$if&lt;/span&gt; one of them was more likely to launch a rug?</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -803,7 +815,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -820,7 +832,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -837,7 +849,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -854,7 +866,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -862,7 +874,7 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" si="1"/>
-        <v>wat &lt;span class='ifOrangeColor'&gt;$if&lt;/span&gt; you could choose the next Binance listing??</v>
+        <v>wat &lt;span class='ifOrangeColor'&gt;$if&lt;/span&gt; you could choose the next Binance listing?</v>
       </c>
     </row>
   </sheetData>
@@ -872,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A986139-330D-43C7-B852-0F4329F65909}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,8 +927,8 @@
         <v>8</v>
       </c>
       <c r="E2" t="str">
-        <f>_xlfn.CONCAT("/images/",C2,".",D2)</f>
-        <v>/images/elon.jpg</v>
+        <f>_xlfn.CONCAT("images/",C2,".",D2)</f>
+        <v>images/elon.jpg</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -933,8 +945,8 @@
         <v>8</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E6" si="0">_xlfn.CONCAT("/images/",C3,".",D3)</f>
-        <v>/images/vitalik.jpg</v>
+        <f t="shared" ref="E3:E59" si="0">_xlfn.CONCAT("images/",C3,".",D3)</f>
+        <v>images/vitalik.jpg</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -952,7 +964,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>/images/trump.jpg</v>
+        <v>images/trump.jpg</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -970,7 +982,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>/images/mitch.jpg</v>
+        <v>images/mitch.jpg</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -988,7 +1000,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>/images/lyxe.jpg</v>
+        <v>images/lyxe.jpg</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -996,17 +1008,17 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
       <c r="E7" t="str">
-        <f t="shared" ref="E7:E38" si="1">_xlfn.CONCAT("/images/",C7,".",D7)</f>
-        <v>/images/kamala.jpeg</v>
+        <f t="shared" si="0"/>
+        <v>images/kamala.jpeg</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1014,17 +1026,17 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/jakey.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/jakey.jpg</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1032,17 +1044,17 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/mrpunk.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mrpunk.jpg</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1050,17 +1062,17 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/patty.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/patty.jpg</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1068,17 +1080,17 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/ansem.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/ansem.jpg</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1086,17 +1098,17 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/daumen.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/daumen.jpg</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1104,17 +1116,17 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/sugar.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/sugar.jpg</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1122,17 +1134,17 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/mememe.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mememe.jpg</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1140,17 +1152,17 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/erik.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/erik.jpg</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1158,17 +1170,17 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/joji.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/joji.jpg</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1176,17 +1188,17 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/a1lon.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/a1lon.jpg</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1194,17 +1206,17 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
         <v>47</v>
       </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/crash.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/crash.jpg</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1212,17 +1224,17 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/dior.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/dior.jpg</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1230,17 +1242,17 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/solstice.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/solstice.jpg</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1248,17 +1260,17 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/pelosi.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/pelosi.jpg</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1266,17 +1278,17 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/buffett.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/buffett.jpg</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1284,17 +1296,17 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ref="E23:E25" si="2">_xlfn.CONCAT("/images/",C23,".",D23)</f>
-        <v>/images/ansem.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/ansem.jpg</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1311,8 +1323,8 @@
         <v>8</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="2"/>
-        <v>/images/mitch.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mitch.jpg</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1329,8 +1341,8 @@
         <v>8</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="2"/>
-        <v>/images/lyxe.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/lyxe.jpg</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1338,17 +1350,17 @@
         <v>17</v>
       </c>
       <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" t="s">
-        <v>48</v>
-      </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" ref="E26" si="3">_xlfn.CONCAT("/images/",C26,".",D26)</f>
-        <v>/images/crash.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/crash.jpg</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,556 +1368,593 @@
         <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="s">
-        <v>79</v>
+      <c r="E27" t="str">
+        <f t="shared" si="0"/>
+        <v>images/burry.jpg</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/invisible.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/cristiano.jpg</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/flying.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/sophie.jpg</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/timetravel.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/livvy.jpg</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/g63.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mrBeast.jpg</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/gt3rs.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/speed.jpg</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/svj.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/g63.jpg</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/enzo.png</v>
+        <f t="shared" si="0"/>
+        <v>images/gt3rs.jpg</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/chiron.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/svj.jpg</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/zonda.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/enzo.png</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/mitch.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/chiron.jpg</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D38" t="s">
         <v>8</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="1"/>
-        <v>/images/lyxe.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/zonda.jpg</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D39" t="s">
         <v>8</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" ref="E39:E49" si="4">_xlfn.CONCAT("/images/",C39,".",D39)</f>
-        <v>/images/jakey.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mitch.jpg</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D40" t="s">
         <v>8</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/punk.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/lyxe.jpg</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
         <v>8</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/patty.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/jakey.jpg</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C42" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D42" t="s">
         <v>8</v>
       </c>
       <c r="E42" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/ansem.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/punk.jpg</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D43" t="s">
         <v>8</v>
       </c>
       <c r="E43" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/daumen.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/patty.jpg</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D44" t="s">
         <v>8</v>
       </c>
       <c r="E44" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/sugar.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/ansem.jpg</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D45" t="s">
         <v>8</v>
       </c>
       <c r="E45" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/mememe.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/daumen.jpg</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
         <v>8</v>
       </c>
       <c r="E46" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/erik.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/sugar.jpg</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D47" t="s">
         <v>8</v>
       </c>
       <c r="E47" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/joji.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mememe.jpg</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
         <v>8</v>
       </c>
       <c r="E48" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/dior.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/erik.jpg</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D49" t="s">
         <v>8</v>
       </c>
       <c r="E49" t="str">
-        <f t="shared" si="4"/>
-        <v>/images/solstice.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/joji.jpg</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>49</v>
       </c>
       <c r="D50" t="s">
         <v>8</v>
       </c>
       <c r="E50" t="str">
-        <f t="shared" ref="E50:E57" si="5">_xlfn.CONCAT("/images/",C50,".",D50)</f>
-        <v>/images/rug.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/dior.jpg</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>86</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>51</v>
       </c>
       <c r="D51" t="s">
         <v>8</v>
       </c>
       <c r="E51" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/runner.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/solstice.jpg</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
       </c>
       <c r="E52" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/mev.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/rug.jpg</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="D53" t="s">
-        <v>68</v>
+        <v>8</v>
       </c>
       <c r="E53" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/griffain.png</v>
+        <f t="shared" si="0"/>
+        <v>images/runner.jpg</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" t="s">
         <v>83</v>
       </c>
-      <c r="B54" t="s">
-        <v>94</v>
-      </c>
-      <c r="C54" t="s">
-        <v>95</v>
-      </c>
       <c r="D54" t="s">
         <v>8</v>
       </c>
       <c r="E54" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/alch.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/mev.jpg</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E55" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/retardio.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/griffain.png</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C56" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>
       </c>
       <c r="E56" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/mother.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/alch.jpg</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C57" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D57" t="s">
         <v>8</v>
       </c>
       <c r="E57" t="str">
-        <f t="shared" si="5"/>
-        <v>/images/GIGA.jpg</v>
+        <f t="shared" si="0"/>
+        <v>images/retardio.jpg</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>images/mother.jpg</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>images/GIGA.jpg</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
images, fallback options for font
</commit_message>
<xml_diff>
--- a/qNa.xlsx
+++ b/qNa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\nodeJS Projects\question-game-mongo\question-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452E3474-7C1E-4946-BFBF-3850DCEEAF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3A17D0-24ED-40F9-920D-215BAFF26A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{B5493750-8CEC-4764-89FF-16A24E89CE02}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="105">
   <si>
     <t>you could go to dinner with one of them</t>
   </si>
@@ -316,9 +316,6 @@
   </si>
   <si>
     <t>GIGA</t>
-  </si>
-  <si>
-    <t>mrpunk</t>
   </si>
   <si>
     <t>you could choose the next Binance listing</t>
@@ -798,7 +795,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -866,7 +863,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -886,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A986139-330D-43C7-B852-0F4329F65909}">
   <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,14 +1044,14 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>93</v>
+        <v>28</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>images/mrpunk.jpg</v>
+        <v>images/punk.jpg</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1386,10 +1383,10 @@
         <v>33</v>
       </c>
       <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
@@ -1404,10 +1401,10 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
-      </c>
-      <c r="C29" t="s">
-        <v>99</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
@@ -1422,10 +1419,10 @@
         <v>33</v>
       </c>
       <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
         <v>100</v>
-      </c>
-      <c r="C30" t="s">
-        <v>101</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
@@ -1440,10 +1437,10 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
         <v>102</v>
-      </c>
-      <c r="C31" t="s">
-        <v>103</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
@@ -1458,10 +1455,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
added tally for majority votes
</commit_message>
<xml_diff>
--- a/qNa.xlsx
+++ b/qNa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\nodeJS Projects\question-game-mongo\question-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FA32CD-B11A-4641-BE0C-7598604E6DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D68583B-33AF-4FA5-B6DB-D16F6A860D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{B5493750-8CEC-4764-89FF-16A24E89CE02}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{B5493750-8CEC-4764-89FF-16A24E89CE02}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE05C373-7301-457B-97A9-2E78D5550DAF}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1076,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A986139-330D-43C7-B852-0F4329F65909}">
   <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2158,11 +2158,11 @@
         <v>106</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
-        <v>images/apple.jpg</v>
+        <v>images/apple.JPG</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
fixed mobile font for majority voting
</commit_message>
<xml_diff>
--- a/qNa.xlsx
+++ b/qNa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\nodeJS Projects\question-game-mongo\question-game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D68583B-33AF-4FA5-B6DB-D16F6A860D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F652BAC-B8B9-491A-8291-004F1E5D85DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="1" xr2:uid="{B5493750-8CEC-4764-89FF-16A24E89CE02}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="153">
   <si>
     <t>you could go to dinner with one of them</t>
   </si>
@@ -543,7 +543,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1074,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A986139-330D-43C7-B852-0F4329F65909}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2323,7 +2334,7 @@
         <v>8</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" ref="E69:E99" si="1">_xlfn.CONCAT("images/",C69,".",D69)</f>
+        <f t="shared" ref="E69:E97" si="1">_xlfn.CONCAT("images/",C69,".",D69)</f>
         <v>images/trump.jpg</v>
       </c>
     </row>
@@ -2584,17 +2595,17 @@
         <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>127</v>
       </c>
       <c r="D84" t="s">
         <v>8</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="1"/>
-        <v>images/lyxe.jpg</v>
+        <v>images/mezoteric.jpg</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2602,17 +2613,17 @@
         <v>122</v>
       </c>
       <c r="B85" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="C85" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
       <c r="D85" t="s">
         <v>8</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="1"/>
-        <v>images/crash.jpg</v>
+        <v>images/kook.jpg</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2620,53 +2631,53 @@
         <v>122</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C86" t="s">
-        <v>127</v>
+        <v>91</v>
       </c>
       <c r="D86" t="s">
         <v>8</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="1"/>
-        <v>images/mezoteric.jpg</v>
+        <v>images/mother.jpg</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C87" t="s">
-        <v>129</v>
+        <v>91</v>
       </c>
       <c r="D87" t="s">
         <v>8</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="1"/>
-        <v>images/kook.jpg</v>
+        <v>images/mother.jpg</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B88" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C88" t="s">
-        <v>91</v>
+        <v>134</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="1"/>
-        <v>images/mother.jpg</v>
+        <v>images/wif.png</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2674,17 +2685,17 @@
         <v>123</v>
       </c>
       <c r="B89" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C89" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="1"/>
-        <v>images/mother.jpg</v>
+        <v>images/popcat.png</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2692,17 +2703,17 @@
         <v>123</v>
       </c>
       <c r="B90" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C90" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D90" t="s">
         <v>61</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="1"/>
-        <v>images/wif.png</v>
+        <v>images/tiktok.png</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2710,17 +2721,17 @@
         <v>123</v>
       </c>
       <c r="B91" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="C91" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D91" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="1"/>
-        <v>images/popcat.png</v>
+        <v>images/ai.jpg</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2728,17 +2739,17 @@
         <v>123</v>
       </c>
       <c r="B92" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C92" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D92" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="1"/>
-        <v>images/tiktok.png</v>
+        <v>images/fart.jpg</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2746,17 +2757,17 @@
         <v>123</v>
       </c>
       <c r="B93" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C93" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D93" t="s">
         <v>8</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="1"/>
-        <v>images/ai.jpg</v>
+        <v>images/racism.jpg</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2764,17 +2775,17 @@
         <v>123</v>
       </c>
       <c r="B94" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D94" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="1"/>
-        <v>images/fart.jpg</v>
+        <v>images/boden.jpeg</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2782,17 +2793,17 @@
         <v>123</v>
       </c>
       <c r="B95" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C95" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D95" t="s">
         <v>8</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="1"/>
-        <v>images/racism.jpg</v>
+        <v>images/wifhat.jpg</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2800,17 +2811,17 @@
         <v>123</v>
       </c>
       <c r="B96" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C96" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D96" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="1"/>
-        <v>images/boden.jpeg</v>
+        <v>images/pepe.jpg</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -2818,57 +2829,24 @@
         <v>123</v>
       </c>
       <c r="B97" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C97" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="1"/>
-        <v>images/wifhat.jpg</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A98" t="s">
-        <v>123</v>
-      </c>
-      <c r="B98" t="s">
-        <v>149</v>
-      </c>
-      <c r="C98" t="s">
-        <v>150</v>
-      </c>
-      <c r="D98" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" t="str">
-        <f t="shared" si="1"/>
-        <v>images/pepe.jpg</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" t="s">
-        <v>123</v>
-      </c>
-      <c r="B99" t="s">
-        <v>151</v>
-      </c>
-      <c r="C99" t="s">
-        <v>152</v>
-      </c>
-      <c r="D99" t="s">
-        <v>61</v>
-      </c>
-      <c r="E99" t="str">
         <f t="shared" si="1"/>
         <v>images/if.png</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B68:B86">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>